<commit_message>
ACTUALIZACION DE LOS DATOS
</commit_message>
<xml_diff>
--- a/Base de datos/Diccionario de datos.xlsx
+++ b/Base de datos/Diccionario de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Reto Final\Base de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0341AF7-AD61-401B-AA5E-40E577103764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EADEFAE-5040-4E5E-86F0-32EAD01085BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo Relacional" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="61">
   <si>
     <t>Inserta aquí una captura con la imagen del modelo relacional</t>
   </si>
@@ -86,97 +86,19 @@
     <t>Cliente</t>
   </si>
   <si>
-    <t>Id_cliente</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>contraseña</t>
-  </si>
-  <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>nacionalidad</t>
-  </si>
-  <si>
-    <t>telefono</t>
-  </si>
-  <si>
-    <t>Id_direccion</t>
-  </si>
-  <si>
     <t>Pedido</t>
-  </si>
-  <si>
-    <t>id_pedido</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>notas</t>
-  </si>
-  <si>
-    <t>producto</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>id_metodo_pago</t>
-  </si>
-  <si>
-    <t>id_direccion</t>
   </si>
   <si>
     <t>Producto</t>
   </si>
   <si>
-    <t>id_producto</t>
-  </si>
-  <si>
-    <t>ingredientes</t>
-  </si>
-  <si>
-    <t>id_categoria</t>
-  </si>
-  <si>
     <t>Lineas_pedido</t>
-  </si>
-  <si>
-    <t>id_lineas_pedido</t>
-  </si>
-  <si>
-    <t>cantidad</t>
   </si>
   <si>
     <t>Direcciones</t>
   </si>
   <si>
-    <t>calle</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>piso</t>
-  </si>
-  <si>
-    <t>cp number</t>
-  </si>
-  <si>
     <t>Metodo_pago</t>
-  </si>
-  <si>
-    <t>efectivo</t>
-  </si>
-  <si>
-    <t>tarjeta</t>
   </si>
   <si>
     <t>x</t>
@@ -185,13 +107,7 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>nombre_categoria</t>
-  </si>
-  <si>
     <t>varchar2</t>
-  </si>
-  <si>
-    <t>char</t>
   </si>
   <si>
     <t>number</t>
@@ -200,18 +116,118 @@
     <t>date</t>
   </si>
   <si>
-    <t>descripcion</t>
+    <t>CLIENTE_ID</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>CREDIT_CARD_NUMBER</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>ADDRESS_ID</t>
+  </si>
+  <si>
+    <t>ORDER_ID INT</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>ORDER_ID</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>ORDER_DATE</t>
+  </si>
+  <si>
+    <t>PAY_METHOD_ID</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>PRODUCT_ID</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>CATEGORY_ID</t>
+  </si>
+  <si>
+    <t>ORDER_LINES_ID</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>CATEGORY_NAME</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>CHAR</t>
+  </si>
+  <si>
+    <t>STREET</t>
+  </si>
+  <si>
+    <t>FLAT</t>
+  </si>
+  <si>
+    <t>POSTAL_CODE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,12 +264,17 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -558,76 +579,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1847,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1870,16 +1898,16 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="3" t="s">
@@ -1888,25 +1916,25 @@
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="6" spans="1:10" ht="21">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75">
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1939,17 +1967,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>53</v>
+      <c r="A8" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
         <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1959,11 +1987,11 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>53</v>
+      <c r="A9" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="12">
         <v>30</v>
@@ -1971,7 +1999,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -1979,11 +2007,11 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>54</v>
+      <c r="A10" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="12">
         <v>30</v>
@@ -1991,7 +2019,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -1999,11 +2027,11 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>53</v>
+      <c r="A11" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="C11" s="25">
         <v>30</v>
@@ -2011,7 +2039,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="25" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -2019,32 +2047,34 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>54</v>
+      <c r="A12" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="25">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>53</v>
+      <c r="A13" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C13" s="12">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
@@ -2055,14 +2085,14 @@
       <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>55</v>
+      <c r="A14" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="12">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -2073,18 +2103,18 @@
       <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>55</v>
+      <c r="A15" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C15" s="12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -2208,110 +2238,110 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -3283,11 +3313,6 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:H34"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="C2:J2"/>
@@ -3295,9 +3320,14 @@
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3306,7 +3336,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3327,42 +3357,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" thickBot="1"/>
     <row r="6" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -3397,17 +3427,17 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -3417,19 +3447,19 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="A9" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>55</v>
+      <c r="A9" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="12">
-        <v>5.2</v>
+        <v>20</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="43" t="s">
-        <v>50</v>
+      <c r="F9" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -3437,14 +3467,14 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1">
-      <c r="A10" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="12">
-        <v>100</v>
+      <c r="A10" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>48</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -3455,19 +3485,19 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="A11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>53</v>
+      <c r="A11" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="C11" s="25">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="43" t="s">
-        <v>50</v>
+      <c r="F11" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -3475,17 +3505,17 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1">
-      <c r="A12" s="24" t="s">
-        <v>32</v>
+      <c r="A12" s="44" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
-      <c r="F12" s="44" t="s">
-        <v>50</v>
+      <c r="F12" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
@@ -3493,18 +3523,18 @@
       <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
-      <c r="A13" s="24" t="s">
-        <v>33</v>
+      <c r="A13" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C13" s="12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -3513,18 +3543,18 @@
       <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1">
-      <c r="A14" s="24" t="s">
-        <v>34</v>
+      <c r="A14" s="44" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="C14" s="12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -3547,7 +3577,7 @@
     <row r="16" spans="1:10" ht="15" customHeight="1">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
@@ -3660,110 +3690,110 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -4758,7 +4788,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4776,42 +4806,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -4846,17 +4876,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -4866,11 +4896,11 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="42" t="s">
-        <v>20</v>
+      <c r="A9" s="44" t="s">
+        <v>50</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C9" s="12">
         <v>30</v>
@@ -4878,7 +4908,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -4886,19 +4916,19 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>37</v>
+      <c r="A10" s="44" t="s">
+        <v>51</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C10" s="12">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -4906,11 +4936,11 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>55</v>
+      <c r="A11" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>47</v>
       </c>
       <c r="C11" s="25">
         <v>5.2</v>
@@ -4918,7 +4948,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="25" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -4926,18 +4956,18 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>55</v>
+      <c r="A12" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="25">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -4946,19 +4976,13 @@
       <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="25">
-        <v>300</v>
-      </c>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -5105,110 +5129,110 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -5236,8 +5260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB348CB6-6937-4E88-A7C8-7EBA68881BA3}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5255,42 +5279,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -5325,17 +5349,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
         <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -5345,18 +5369,18 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>55</v>
+      <c r="A9" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>37</v>
       </c>
       <c r="C9" s="12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -5365,18 +5389,18 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>55</v>
+      <c r="A10" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="12">
         <v>20</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -5385,19 +5409,19 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>55</v>
+      <c r="A11" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="25">
         <v>20</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="43" t="s">
-        <v>50</v>
+      <c r="F11" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -5568,110 +5592,110 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -5699,7 +5723,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5717,42 +5741,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -5787,17 +5811,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -5807,19 +5831,19 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>53</v>
+      <c r="A9" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="12">
         <v>20</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>50</v>
+      <c r="F9" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -6014,110 +6038,110 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -6144,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86DF4C8E-D136-434D-A403-9F984396D828}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6163,42 +6187,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -6233,17 +6257,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -6253,38 +6277,32 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>55</v>
+      <c r="A9" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="C9" s="12">
-        <v>5.2</v>
+        <v>2</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="12">
-        <v>16</v>
-      </c>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -6466,110 +6484,110 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>
@@ -6596,8 +6614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C434550-99C9-417C-8D16-BFAE91B799A1}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6617,42 +6635,42 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B3" s="23">
         <v>44693</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="19.5" thickBot="1">
       <c r="A7" s="4" t="s">
@@ -6687,17 +6705,17 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>55</v>
+      <c r="A8" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="C8" s="9">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -6707,11 +6725,11 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>53</v>
+      <c r="A9" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="12">
         <v>30</v>
@@ -6719,7 +6737,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -6727,19 +6745,19 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>55</v>
+      <c r="A10" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="12">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="25" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -6747,35 +6765,27 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>54</v>
+      <c r="A11" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="25">
         <v>10</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="25" t="s">
-        <v>50</v>
-      </c>
+      <c r="F11" s="25"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="25">
-        <v>10</v>
-      </c>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -6936,110 +6946,110 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="43"/>
       <c r="I26" s="10"/>
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="13"/>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="13"/>
       <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="13"/>
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="13"/>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="13"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="26"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="13"/>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="13"/>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
       <c r="I34" s="16"/>
       <c r="J34" s="22"/>
     </row>

</xml_diff>